<commit_message>
3th commit - change excel file
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam\OneDrive - Seneca\Desktop\HTML projects - Copy\testing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD804910-6736-431C-96F3-CD62A8A0E621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,37 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>Testing file</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>ads</t>
+  </si>
+  <si>
+    <t>das</t>
+  </si>
+  <si>
+    <t>dsa</t>
+  </si>
+  <si>
+    <t>asdsda</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +368,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="Q12:Y33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="12" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+    </row>
+    <row r="13" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+    </row>
+    <row r="14" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+    </row>
+    <row r="15" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+    </row>
+    <row r="16" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+    </row>
+    <row r="17" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+    </row>
+    <row r="18" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+    </row>
+    <row r="19" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+    </row>
+    <row r="20" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+    </row>
+    <row r="21" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+    </row>
+    <row r="22" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+    </row>
+    <row r="23" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+    </row>
+    <row r="26" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="17:25" x14ac:dyDescent="0.25">
+      <c r="Q32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Q12:Y23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>